<commit_message>
Se agrega pantalla para configurar la conversion analogo digital. Se agrega pantalla para activar componentes adicionales. Se mejora presentacion en varias pantallas.
</commit_message>
<xml_diff>
--- a/Pruebas/conversion adc.xlsx
+++ b/Pruebas/conversion adc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>°c</t>
   </si>
@@ -25,6 +25,18 @@
   </si>
   <si>
     <t>°F</t>
+  </si>
+  <si>
+    <t>sub</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>mul</t>
+  </si>
+  <si>
+    <t>add</t>
   </si>
 </sst>
 </file>
@@ -66,7 +78,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -363,15 +386,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -382,18 +405,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1544</v>
       </c>
       <c r="C2">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D2">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>B2</f>
+        <v>1544</v>
+      </c>
+      <c r="I2">
+        <f>C2*K2</f>
+        <v>2050000</v>
+      </c>
+      <c r="K2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>892</v>
       </c>
@@ -403,22 +437,145 @@
       <c r="D3">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>B3</f>
+        <v>892</v>
+      </c>
+      <c r="I3">
+        <f>C3*K2</f>
+        <v>536000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f>B6</f>
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>1434</v>
+        <v>2204</v>
       </c>
       <c r="C6">
         <f>FORECAST(B6,C2:C3,B2:B3)</f>
-        <v>177.7944785276074</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>358.25766871165649</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <f>I2</f>
+        <v>2050000</v>
+      </c>
+      <c r="H6">
+        <f>I3</f>
+        <v>536000</v>
+      </c>
+      <c r="I6">
+        <f>TRUNC(G6-H6)</f>
+        <v>1514000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f>H2</f>
+        <v>1544</v>
+      </c>
+      <c r="H7">
+        <f>H3</f>
+        <v>892</v>
+      </c>
+      <c r="I7">
+        <f>TRUNC(G7-H7)</f>
+        <v>652</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f>I6</f>
+        <v>1514000</v>
+      </c>
+      <c r="H8">
+        <f>I7</f>
+        <v>652</v>
+      </c>
+      <c r="I8">
+        <f>TRUNC(G8/H8)</f>
+        <v>2322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <f>H4</f>
+        <v>2204</v>
+      </c>
+      <c r="H9">
+        <f>H3</f>
+        <v>892</v>
+      </c>
+      <c r="I9">
+        <f>TRUNC(G9-H9)</f>
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <f>I8</f>
+        <v>2322</v>
+      </c>
+      <c r="H10">
+        <f>I9</f>
+        <v>1312</v>
+      </c>
+      <c r="I10">
+        <f>TRUNC(G10*H10)</f>
+        <v>3046464</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <f>I10</f>
+        <v>3046464</v>
+      </c>
+      <c r="H11">
+        <f>I3</f>
+        <v>536000</v>
+      </c>
+      <c r="I11">
+        <f>TRUNC(G11+H11)</f>
+        <v>3582464</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>798</v>
       </c>
+      <c r="I13">
+        <f>TRUNC(I11/K2)</f>
+        <v>358</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G6:I11">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>65535</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>